<commit_message>
now saving linecount and startline in meta
</commit_message>
<xml_diff>
--- a/parallel/Parallel Concepts/Aufteilung.xlsx
+++ b/parallel/Parallel Concepts/Aufteilung.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$B$6" max="4" min="1" page="10" val="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$B$6" max="4" min="1" page="10" val="2"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,7 +696,7 @@
   <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,15 +815,15 @@
     </row>
     <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="16">
         <f>ROUNDDOWN(B5/B6,0)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D6" s="17">
         <f>MOD(B5,B6)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="C8" s="10">
         <f>IF(B8&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" s="8">
         <f>B8*$C$6+E8</f>
@@ -864,11 +864,11 @@
       </c>
       <c r="C9" s="10">
         <f>IF(B9&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8">
         <f>B9*$C$6+E9</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2">
         <f>MIN($D$6,B9)</f>
@@ -881,15 +881,15 @@
       </c>
       <c r="C10" s="10">
         <f>IF(B10&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" s="8">
         <f>B10*$C$6+E10</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ref="E10:E11" si="0">MIN($D$6,B10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -898,15 +898,15 @@
       </c>
       <c r="C11" s="11">
         <f>IF(B11&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D11" s="9">
         <f>B11*$C$6+E11</f>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no clue what im doing, added alot for switching process
</commit_message>
<xml_diff>
--- a/parallel/Parallel Concepts/Aufteilung.xlsx
+++ b/parallel/Parallel Concepts/Aufteilung.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09728d54189c9567/UNI/Praktikum/PAPO_SS2017/parallel/Parallel Concepts/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="392" documentId="0C5EC25F90779C07A51A19F0A185B989CCAE0E43" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{D3049C05-3FAE-4E6B-AAE8-6B6CF0FC262A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11070" windowHeight="10155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11076" windowHeight="10152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,8 +49,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +82,128 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -191,11 +305,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -230,24 +419,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -270,6 +497,48 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -284,11 +553,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$B$5" max="30" min="10" page="10" val="23"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$R$3" max="300" min="10" page="10" val="64"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$B$6" max="4" min="1" page="10" val="2"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$R$4" max="19" min="1" page="10" val="3"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -297,16 +566,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>581025</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>579120</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>752475</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>754380</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>259080</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -316,7 +585,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D07E0B-27AA-4D66-B6EC-D75B98300467}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -347,16 +616,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>266699</xdr:rowOff>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>7620</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>266700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>190501</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>257174</xdr:rowOff>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>259080</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -366,7 +635,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3BA0196-BD28-485F-92F1-532EECE31030}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -397,7 +666,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -692,240 +961,1853 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="V7" sqref="V7:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="R3" s="15">
+        <v>64</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="28"/>
+    </row>
+    <row r="4" spans="1:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="R4" s="14">
+        <v>3</v>
+      </c>
+      <c r="S4" s="16">
+        <f>ROUNDDOWN(R3/R4,0)</f>
+        <v>21</v>
+      </c>
+      <c r="T4" s="17">
+        <f>MOD(R3,R4)</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="29">
+        <v>1</v>
+      </c>
+      <c r="W4" s="30">
+        <v>2</v>
+      </c>
+      <c r="X4" s="30">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="30">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="R5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="T5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="32">
+        <f>-Z5-1</f>
+        <v>-1</v>
+      </c>
+      <c r="W5" s="33">
+        <f>-Z5</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="43">
+        <v>-1</v>
+      </c>
+      <c r="Y5" s="43">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="33">
+        <f>TRUNC(16/S4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="34">
+        <f>Z5+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G6">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="H6">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="I6">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="J6">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="K6">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="L6">
         <v>11</v>
       </c>
-      <c r="M2">
+      <c r="M6">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="N6">
         <v>13</v>
       </c>
-      <c r="O2">
+      <c r="O6">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="P6">
         <v>15</v>
       </c>
+      <c r="R6" s="50">
+        <v>0</v>
+      </c>
+      <c r="S6" s="10">
+        <f>IF(R6&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>22</v>
+      </c>
+      <c r="T6" s="8">
+        <f>R6*$S$4+U6</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <f>MIN($T$4,R6)</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="26">
+        <f>$R6+V$5</f>
+        <v>-1</v>
+      </c>
+      <c r="W6" s="27">
+        <f>$R6+W5</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="42">
+        <f>$R6+X5</f>
+        <v>-1</v>
+      </c>
+      <c r="Y6" s="42">
+        <f t="shared" ref="X6:AA6" si="0">$R6+Y5</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>16</v>
       </c>
-      <c r="B3">
+      <c r="B7">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="C7">
         <v>18</v>
       </c>
-      <c r="D3">
+      <c r="D7">
         <v>19</v>
       </c>
-      <c r="E3">
+      <c r="E7">
         <v>20</v>
       </c>
-      <c r="F3">
+      <c r="F7">
         <v>21</v>
       </c>
-      <c r="G3">
+      <c r="G7">
         <v>22</v>
       </c>
-      <c r="H3">
+      <c r="H7">
         <v>23</v>
       </c>
-      <c r="I3">
+      <c r="I7" s="22">
         <v>24</v>
       </c>
-      <c r="J3">
+      <c r="J7" s="22">
         <v>25</v>
       </c>
-      <c r="K3">
+      <c r="K7" s="22">
         <v>26</v>
       </c>
-      <c r="L3">
+      <c r="L7" s="23">
         <v>27</v>
       </c>
-      <c r="M3">
+      <c r="M7" s="23">
         <v>28</v>
       </c>
-      <c r="N3">
+      <c r="N7" s="23">
         <v>29</v>
       </c>
-      <c r="O3">
+      <c r="O7" s="24">
         <v>30</v>
       </c>
-      <c r="P3">
+      <c r="P7" s="24">
         <v>31</v>
       </c>
+      <c r="R7" s="47">
+        <v>1</v>
+      </c>
+      <c r="S7" s="10">
+        <f>IF(R7&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T7" s="8">
+        <f>R7*$S$4+U7</f>
+        <v>22</v>
+      </c>
+      <c r="U7" s="2">
+        <f>MIN($T$4,R7)</f>
+        <v>1</v>
+      </c>
+      <c r="V7" s="35">
+        <f>$R7+V$5</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="36">
+        <f>$R7+W$5</f>
+        <v>1</v>
+      </c>
+      <c r="X7" s="44">
+        <f t="shared" ref="X7:AA22" si="1">$R7+X$5</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Z7" s="38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AA7" s="37">
+        <f>$R7+AA$5</f>
+        <v>2</v>
+      </c>
+      <c r="AD7">
+        <f>TRUNC(AD6 / $R$3*$S$4,0)</f>
+        <v>7</v>
+      </c>
+      <c r="AE7" t="b">
+        <f>AD7&lt;T4</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="15">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>32</v>
+      </c>
+      <c r="B8" s="25">
+        <v>33</v>
+      </c>
+      <c r="C8" s="25">
+        <v>34</v>
+      </c>
+      <c r="D8" s="25">
+        <v>35</v>
+      </c>
+      <c r="E8" s="20">
+        <v>36</v>
+      </c>
+      <c r="F8" s="20">
+        <v>37</v>
+      </c>
+      <c r="G8" s="20">
+        <v>38</v>
+      </c>
+      <c r="H8" s="21">
+        <v>39</v>
+      </c>
+      <c r="I8" s="18">
+        <v>40</v>
+      </c>
+      <c r="J8" s="18">
+        <v>41</v>
+      </c>
+      <c r="K8" s="18">
+        <v>42</v>
+      </c>
+      <c r="L8" s="55">
+        <v>43</v>
+      </c>
+      <c r="M8" s="55">
+        <v>44</v>
+      </c>
+      <c r="N8" s="55">
+        <v>45</v>
+      </c>
+      <c r="O8" s="55">
+        <v>46</v>
+      </c>
+      <c r="P8" s="55">
+        <v>47</v>
+      </c>
+      <c r="R8" s="49">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="S8" s="10">
+        <f>IF(R8&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T8" s="8">
+        <f>R8*$S$4+U8</f>
+        <v>43</v>
+      </c>
+      <c r="U8" s="2">
+        <f>MIN($T$4,R8)</f>
+        <v>1</v>
+      </c>
+      <c r="V8" s="35">
+        <f t="shared" ref="V8:AA25" si="2">$R8+V$5</f>
+        <v>1</v>
+      </c>
+      <c r="W8" s="36">
+        <f>$R8+W$5</f>
+        <v>2</v>
+      </c>
+      <c r="X8" s="44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Y8" s="44">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="Z8" s="36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AA8" s="37">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AD8">
+        <f>TRUNC(AD6 / $R$3*($S$4+1),0)</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="14">
+    <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <v>48</v>
+      </c>
+      <c r="B9" s="21">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>51</v>
+      </c>
+      <c r="E9">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>54</v>
+      </c>
+      <c r="H9">
+        <v>55</v>
+      </c>
+      <c r="I9">
+        <v>56</v>
+      </c>
+      <c r="J9">
+        <v>57</v>
+      </c>
+      <c r="K9">
+        <v>58</v>
+      </c>
+      <c r="L9">
+        <v>59</v>
+      </c>
+      <c r="M9">
+        <v>60</v>
+      </c>
+      <c r="N9">
+        <v>61</v>
+      </c>
+      <c r="O9">
+        <v>62</v>
+      </c>
+      <c r="P9">
+        <v>63</v>
+      </c>
+      <c r="R9" s="48">
+        <v>3</v>
+      </c>
+      <c r="S9" s="10">
+        <f>IF(R9&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T9" s="8">
+        <f>R9*$S$4+U9</f>
+        <v>64</v>
+      </c>
+      <c r="U9" s="2">
+        <f>MIN($T$4,R9)</f>
+        <v>1</v>
+      </c>
+      <c r="V9" s="35">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="C6" s="16">
-        <f>ROUNDDOWN(B5/B6,0)</f>
+      <c r="W9" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="X9" s="44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Y9" s="44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Z9" s="36">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AA9" s="37">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>67</v>
+      </c>
+      <c r="E10">
+        <v>68</v>
+      </c>
+      <c r="F10">
+        <v>69</v>
+      </c>
+      <c r="G10">
+        <v>70</v>
+      </c>
+      <c r="H10">
+        <v>71</v>
+      </c>
+      <c r="I10">
+        <v>72</v>
+      </c>
+      <c r="J10">
+        <v>73</v>
+      </c>
+      <c r="K10">
+        <v>74</v>
+      </c>
+      <c r="L10">
+        <v>75</v>
+      </c>
+      <c r="M10">
+        <v>76</v>
+      </c>
+      <c r="N10">
+        <v>77</v>
+      </c>
+      <c r="O10">
+        <v>78</v>
+      </c>
+      <c r="P10">
+        <v>79</v>
+      </c>
+      <c r="R10" s="46">
+        <v>4</v>
+      </c>
+      <c r="S10" s="10">
+        <f>IF(R10&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T10" s="8">
+        <f>R10*$S$4+U10</f>
+        <v>85</v>
+      </c>
+      <c r="U10" s="2">
+        <f>MIN($T$4,R10)</f>
+        <v>1</v>
+      </c>
+      <c r="V10" s="54">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="W10" s="36">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="X10" s="44">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Y10" s="44">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Z10" s="36">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AA10" s="37">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>81</v>
+      </c>
+      <c r="C11">
+        <v>82</v>
+      </c>
+      <c r="D11">
+        <v>83</v>
+      </c>
+      <c r="E11">
+        <v>84</v>
+      </c>
+      <c r="F11">
+        <v>85</v>
+      </c>
+      <c r="G11">
+        <v>86</v>
+      </c>
+      <c r="H11">
+        <v>87</v>
+      </c>
+      <c r="I11">
+        <v>88</v>
+      </c>
+      <c r="J11">
+        <v>89</v>
+      </c>
+      <c r="K11">
+        <v>90</v>
+      </c>
+      <c r="L11">
+        <v>91</v>
+      </c>
+      <c r="M11">
+        <v>92</v>
+      </c>
+      <c r="N11">
+        <v>93</v>
+      </c>
+      <c r="O11">
+        <v>94</v>
+      </c>
+      <c r="P11">
+        <v>95</v>
+      </c>
+      <c r="R11" s="45">
+        <v>5</v>
+      </c>
+      <c r="S11" s="10">
+        <f>IF(R11&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T11" s="8">
+        <f>R11*$S$4+U11</f>
+        <v>106</v>
+      </c>
+      <c r="U11" s="2">
+        <f>MIN($T$4,R11)</f>
+        <v>1</v>
+      </c>
+      <c r="V11" s="54">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="W11" s="36">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="X11" s="44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y11" s="44">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Z11" s="36">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AA11" s="37">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>96</v>
+      </c>
+      <c r="B12">
+        <v>97</v>
+      </c>
+      <c r="C12">
+        <v>98</v>
+      </c>
+      <c r="D12">
+        <v>99</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>101</v>
+      </c>
+      <c r="G12">
+        <v>102</v>
+      </c>
+      <c r="H12">
+        <v>103</v>
+      </c>
+      <c r="I12">
+        <v>104</v>
+      </c>
+      <c r="J12">
+        <v>105</v>
+      </c>
+      <c r="K12">
+        <v>106</v>
+      </c>
+      <c r="L12">
+        <v>107</v>
+      </c>
+      <c r="M12">
+        <v>108</v>
+      </c>
+      <c r="N12">
+        <v>109</v>
+      </c>
+      <c r="O12">
+        <v>110</v>
+      </c>
+      <c r="P12">
+        <v>111</v>
+      </c>
+      <c r="R12" s="51">
+        <v>6</v>
+      </c>
+      <c r="S12" s="10">
+        <f>IF(R12&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T12" s="8">
+        <f>R12*$S$4+U12</f>
+        <v>127</v>
+      </c>
+      <c r="U12" s="2">
+        <f>MIN($T$4,R12)</f>
+        <v>1</v>
+      </c>
+      <c r="V12" s="35">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="W12" s="36">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="X12" s="44">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Y12" s="44">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z12" s="36">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AA12" s="37">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>113</v>
+      </c>
+      <c r="C13">
+        <v>114</v>
+      </c>
+      <c r="D13">
+        <v>115</v>
+      </c>
+      <c r="E13">
+        <v>116</v>
+      </c>
+      <c r="F13">
+        <v>117</v>
+      </c>
+      <c r="G13">
+        <v>118</v>
+      </c>
+      <c r="H13">
+        <v>119</v>
+      </c>
+      <c r="I13">
+        <v>120</v>
+      </c>
+      <c r="J13">
+        <v>121</v>
+      </c>
+      <c r="K13">
+        <v>122</v>
+      </c>
+      <c r="L13">
+        <v>123</v>
+      </c>
+      <c r="M13">
+        <v>124</v>
+      </c>
+      <c r="N13">
+        <v>125</v>
+      </c>
+      <c r="O13">
+        <v>126</v>
+      </c>
+      <c r="P13">
+        <v>127</v>
+      </c>
+      <c r="R13" s="47">
+        <v>7</v>
+      </c>
+      <c r="S13" s="10">
+        <f>IF(R13&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T13" s="8">
+        <f>R13*$S$4+U13</f>
+        <v>148</v>
+      </c>
+      <c r="U13" s="2">
+        <f>MIN($T$4,R13)</f>
+        <v>1</v>
+      </c>
+      <c r="V13" s="35">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="W13" s="36">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="X13" s="44">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Y13" s="44">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Z13" s="36">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AA13" s="37">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>128</v>
+      </c>
+      <c r="B14">
+        <v>129</v>
+      </c>
+      <c r="C14">
+        <v>130</v>
+      </c>
+      <c r="D14">
+        <v>131</v>
+      </c>
+      <c r="E14">
+        <v>132</v>
+      </c>
+      <c r="F14">
+        <v>133</v>
+      </c>
+      <c r="G14">
+        <v>134</v>
+      </c>
+      <c r="H14">
+        <v>135</v>
+      </c>
+      <c r="I14">
+        <v>136</v>
+      </c>
+      <c r="J14">
+        <v>137</v>
+      </c>
+      <c r="K14">
+        <v>138</v>
+      </c>
+      <c r="L14">
+        <v>139</v>
+      </c>
+      <c r="M14">
+        <v>140</v>
+      </c>
+      <c r="N14">
+        <v>141</v>
+      </c>
+      <c r="O14">
+        <v>142</v>
+      </c>
+      <c r="P14">
+        <v>143</v>
+      </c>
+      <c r="R14" s="56">
+        <v>8</v>
+      </c>
+      <c r="S14" s="10">
+        <f>IF(R14&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T14" s="8">
+        <f>R14*$S$4+U14</f>
+        <v>169</v>
+      </c>
+      <c r="U14" s="2">
+        <f>MIN($T$4,R14)</f>
+        <v>1</v>
+      </c>
+      <c r="V14" s="35">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="W14" s="36">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="X14" s="44">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y14" s="44">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Z14" s="36">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AA14" s="37">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>144</v>
+      </c>
+      <c r="B15">
+        <v>145</v>
+      </c>
+      <c r="C15">
+        <v>146</v>
+      </c>
+      <c r="D15">
+        <v>147</v>
+      </c>
+      <c r="E15">
+        <v>148</v>
+      </c>
+      <c r="F15">
+        <v>149</v>
+      </c>
+      <c r="G15">
+        <v>150</v>
+      </c>
+      <c r="H15">
+        <v>151</v>
+      </c>
+      <c r="I15">
+        <v>152</v>
+      </c>
+      <c r="J15">
+        <v>153</v>
+      </c>
+      <c r="K15">
+        <v>154</v>
+      </c>
+      <c r="L15">
+        <v>155</v>
+      </c>
+      <c r="M15">
+        <v>156</v>
+      </c>
+      <c r="N15">
+        <v>157</v>
+      </c>
+      <c r="O15">
+        <v>158</v>
+      </c>
+      <c r="P15">
+        <v>159</v>
+      </c>
+      <c r="R15" s="5">
+        <v>9</v>
+      </c>
+      <c r="S15" s="10">
+        <f>IF(R15&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T15" s="8">
+        <f>R15*$S$4+U15</f>
+        <v>190</v>
+      </c>
+      <c r="U15" s="2">
+        <f>MIN($T$4,R15)</f>
+        <v>1</v>
+      </c>
+      <c r="V15" s="57">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="W15" s="58">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="X15" s="59">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Y15" s="59">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="Z15" s="36">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AA15" s="37">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>160</v>
+      </c>
+      <c r="B16">
+        <v>161</v>
+      </c>
+      <c r="C16">
+        <v>162</v>
+      </c>
+      <c r="D16">
+        <v>163</v>
+      </c>
+      <c r="E16">
+        <v>164</v>
+      </c>
+      <c r="F16">
+        <v>165</v>
+      </c>
+      <c r="G16">
+        <v>166</v>
+      </c>
+      <c r="H16">
+        <v>167</v>
+      </c>
+      <c r="I16">
+        <v>168</v>
+      </c>
+      <c r="J16">
+        <v>169</v>
+      </c>
+      <c r="K16">
+        <v>170</v>
+      </c>
+      <c r="L16">
+        <v>171</v>
+      </c>
+      <c r="M16">
+        <v>172</v>
+      </c>
+      <c r="N16">
+        <v>173</v>
+      </c>
+      <c r="O16">
+        <v>174</v>
+      </c>
+      <c r="P16">
+        <v>175</v>
+      </c>
+      <c r="R16" s="5">
+        <v>10</v>
+      </c>
+      <c r="S16" s="10">
+        <f>IF(R16&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T16" s="8">
+        <f>R16*$S$4+U16</f>
+        <v>211</v>
+      </c>
+      <c r="U16" s="2">
+        <f>MIN($T$4,R16)</f>
+        <v>1</v>
+      </c>
+      <c r="V16" s="57">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="W16" s="58">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="X16" s="59">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Y16" s="59">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D6" s="17">
-        <f>MOD(B5,B6)</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="2"/>
+      <c r="Z16" s="36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AA16" s="37">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>5</v>
-      </c>
+    <row r="17" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <v>177</v>
+      </c>
+      <c r="C17">
+        <v>178</v>
+      </c>
+      <c r="D17">
+        <v>179</v>
+      </c>
+      <c r="E17">
+        <v>180</v>
+      </c>
+      <c r="F17">
+        <v>181</v>
+      </c>
+      <c r="G17">
+        <v>182</v>
+      </c>
+      <c r="H17">
+        <v>183</v>
+      </c>
+      <c r="I17">
+        <v>184</v>
+      </c>
+      <c r="J17">
+        <v>185</v>
+      </c>
+      <c r="K17">
+        <v>186</v>
+      </c>
+      <c r="L17">
+        <v>187</v>
+      </c>
+      <c r="M17">
+        <v>188</v>
+      </c>
+      <c r="N17">
+        <v>189</v>
+      </c>
+      <c r="O17">
+        <v>190</v>
+      </c>
+      <c r="P17">
+        <v>191</v>
+      </c>
+      <c r="R17" s="5">
+        <v>11</v>
+      </c>
+      <c r="S17" s="10">
+        <f>IF(R17&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T17" s="8">
+        <f>R17*$S$4+U17</f>
+        <v>232</v>
+      </c>
+      <c r="U17" s="2">
+        <f>MIN($T$4,R17)</f>
+        <v>1</v>
+      </c>
+      <c r="V17" s="57">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="W17" s="58">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="X17" s="59">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="Y17" s="59">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="Z17" s="36">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="AA17" s="37">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+      <c r="AE17" s="19"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10">
-        <f>IF(B8&lt;$D$6,$C$6+1,$C$6)</f>
+    <row r="18" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>192</v>
+      </c>
+      <c r="B18">
+        <v>193</v>
+      </c>
+      <c r="C18">
+        <v>194</v>
+      </c>
+      <c r="D18">
+        <v>195</v>
+      </c>
+      <c r="E18">
+        <v>196</v>
+      </c>
+      <c r="F18">
+        <v>197</v>
+      </c>
+      <c r="G18">
+        <v>198</v>
+      </c>
+      <c r="H18">
+        <v>199</v>
+      </c>
+      <c r="I18">
+        <v>200</v>
+      </c>
+      <c r="J18">
+        <v>201</v>
+      </c>
+      <c r="K18">
+        <v>202</v>
+      </c>
+      <c r="L18">
+        <v>203</v>
+      </c>
+      <c r="M18">
+        <v>204</v>
+      </c>
+      <c r="N18">
+        <v>205</v>
+      </c>
+      <c r="O18">
+        <v>206</v>
+      </c>
+      <c r="P18">
+        <v>207</v>
+      </c>
+      <c r="R18" s="5">
         <v>12</v>
       </c>
-      <c r="D8" s="8">
-        <f>B8*$C$6+E8</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <f>MIN($D$6,B8)</f>
-        <v>0</v>
-      </c>
+      <c r="S18" s="10">
+        <f>IF(R18&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T18" s="8">
+        <f>R18*$S$4+U18</f>
+        <v>253</v>
+      </c>
+      <c r="U18" s="2">
+        <f>MIN($T$4,R18)</f>
+        <v>1</v>
+      </c>
+      <c r="V18" s="57">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="W18" s="58">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="X18" s="59">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="Y18" s="59">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Z18" s="36">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AA18" s="37">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10">
-        <f>IF(B9&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>11</v>
-      </c>
-      <c r="D9" s="8">
-        <f>B9*$C$6+E9</f>
+    <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>208</v>
+      </c>
+      <c r="B19">
+        <v>209</v>
+      </c>
+      <c r="C19">
+        <v>210</v>
+      </c>
+      <c r="D19">
+        <v>211</v>
+      </c>
+      <c r="E19">
+        <v>212</v>
+      </c>
+      <c r="F19">
+        <v>213</v>
+      </c>
+      <c r="G19">
+        <v>214</v>
+      </c>
+      <c r="H19">
+        <v>215</v>
+      </c>
+      <c r="I19">
+        <v>216</v>
+      </c>
+      <c r="J19">
+        <v>217</v>
+      </c>
+      <c r="K19">
+        <v>218</v>
+      </c>
+      <c r="L19">
+        <v>219</v>
+      </c>
+      <c r="M19">
+        <v>220</v>
+      </c>
+      <c r="N19">
+        <v>221</v>
+      </c>
+      <c r="O19">
+        <v>222</v>
+      </c>
+      <c r="P19">
+        <v>223</v>
+      </c>
+      <c r="R19" s="5">
+        <v>13</v>
+      </c>
+      <c r="S19" s="10">
+        <f>IF(R19&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T19" s="8">
+        <f>R19*$S$4+U19</f>
+        <v>274</v>
+      </c>
+      <c r="U19" s="2">
+        <f>MIN($T$4,R19)</f>
+        <v>1</v>
+      </c>
+      <c r="V19" s="57">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E9" s="2">
-        <f>MIN($D$6,B9)</f>
-        <v>1</v>
-      </c>
+      <c r="W19" s="58">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="X19" s="59">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="Y19" s="59">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="Z19" s="36">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AA19" s="37">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="10">
-        <f>IF(B10&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>11</v>
-      </c>
-      <c r="D10" s="8">
-        <f>B10*$C$6+E10</f>
-        <v>23</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" ref="E10:E11" si="0">MIN($D$6,B10)</f>
-        <v>1</v>
-      </c>
+    <row r="20" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>224</v>
+      </c>
+      <c r="B20">
+        <v>225</v>
+      </c>
+      <c r="C20">
+        <v>226</v>
+      </c>
+      <c r="D20">
+        <v>227</v>
+      </c>
+      <c r="E20">
+        <v>228</v>
+      </c>
+      <c r="F20">
+        <v>229</v>
+      </c>
+      <c r="G20">
+        <v>230</v>
+      </c>
+      <c r="H20">
+        <v>231</v>
+      </c>
+      <c r="I20">
+        <v>232</v>
+      </c>
+      <c r="J20">
+        <v>233</v>
+      </c>
+      <c r="K20">
+        <v>234</v>
+      </c>
+      <c r="L20">
+        <v>235</v>
+      </c>
+      <c r="M20">
+        <v>236</v>
+      </c>
+      <c r="N20">
+        <v>237</v>
+      </c>
+      <c r="O20">
+        <v>238</v>
+      </c>
+      <c r="P20">
+        <v>239</v>
+      </c>
+      <c r="R20" s="5">
+        <v>14</v>
+      </c>
+      <c r="S20" s="10">
+        <f>IF(R20&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T20" s="8">
+        <f>R20*$S$4+U20</f>
+        <v>295</v>
+      </c>
+      <c r="U20" s="2">
+        <f>MIN($T$4,R20)</f>
+        <v>1</v>
+      </c>
+      <c r="V20" s="57">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="W20" s="58">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="X20" s="59">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Y20" s="59">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Z20" s="36">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AA20" s="37">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
+      <c r="AE20" s="19"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>3</v>
-      </c>
-      <c r="C11" s="11">
-        <f>IF(B11&lt;$D$6,$C$6+1,$C$6)</f>
-        <v>11</v>
-      </c>
-      <c r="D11" s="9">
-        <f>B11*$C$6+E11</f>
-        <v>34</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+    <row r="21" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>240</v>
+      </c>
+      <c r="B21">
+        <v>241</v>
+      </c>
+      <c r="C21">
+        <v>242</v>
+      </c>
+      <c r="D21">
+        <v>243</v>
+      </c>
+      <c r="E21">
+        <v>244</v>
+      </c>
+      <c r="F21">
+        <v>245</v>
+      </c>
+      <c r="G21">
+        <v>246</v>
+      </c>
+      <c r="H21">
+        <v>247</v>
+      </c>
+      <c r="I21">
+        <v>248</v>
+      </c>
+      <c r="J21">
+        <v>249</v>
+      </c>
+      <c r="K21">
+        <v>250</v>
+      </c>
+      <c r="L21">
+        <v>251</v>
+      </c>
+      <c r="M21">
+        <v>252</v>
+      </c>
+      <c r="N21">
+        <v>253</v>
+      </c>
+      <c r="O21">
+        <v>254</v>
+      </c>
+      <c r="P21">
+        <v>255</v>
+      </c>
+      <c r="R21" s="5">
+        <v>15</v>
+      </c>
+      <c r="S21" s="10">
+        <f>IF(R21&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T21" s="8">
+        <f>R21*$S$4+U21</f>
+        <v>316</v>
+      </c>
+      <c r="U21" s="2">
+        <f>MIN($T$4,R21)</f>
+        <v>1</v>
+      </c>
+      <c r="V21" s="35">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="W21" s="36">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="X21" s="44">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="Y21" s="44">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="Z21" s="36">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="AA21" s="37">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AD21" s="19"/>
+    </row>
+    <row r="22" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>256</v>
+      </c>
+      <c r="B22">
+        <v>257</v>
+      </c>
+      <c r="C22">
+        <v>258</v>
+      </c>
+      <c r="D22">
+        <v>259</v>
+      </c>
+      <c r="E22">
+        <v>260</v>
+      </c>
+      <c r="F22">
+        <v>261</v>
+      </c>
+      <c r="G22">
+        <v>262</v>
+      </c>
+      <c r="H22">
+        <v>263</v>
+      </c>
+      <c r="I22">
+        <v>264</v>
+      </c>
+      <c r="J22">
+        <v>265</v>
+      </c>
+      <c r="K22">
+        <v>266</v>
+      </c>
+      <c r="L22">
+        <v>267</v>
+      </c>
+      <c r="M22">
+        <v>268</v>
+      </c>
+      <c r="N22">
+        <v>269</v>
+      </c>
+      <c r="O22">
+        <v>270</v>
+      </c>
+      <c r="P22">
+        <v>271</v>
+      </c>
+      <c r="R22" s="5">
+        <v>16</v>
+      </c>
+      <c r="S22" s="10">
+        <f>IF(R22&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T22" s="8">
+        <f>R22*$S$4+U22</f>
+        <v>337</v>
+      </c>
+      <c r="U22" s="2">
+        <f>MIN($T$4,R22)</f>
+        <v>1</v>
+      </c>
+      <c r="V22" s="35">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="W22" s="36">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="X22" s="44">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Y22" s="44">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="Z22" s="36">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AA22" s="37">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>272</v>
+      </c>
+      <c r="B23">
+        <v>273</v>
+      </c>
+      <c r="C23">
+        <v>274</v>
+      </c>
+      <c r="D23">
+        <v>275</v>
+      </c>
+      <c r="E23">
+        <v>276</v>
+      </c>
+      <c r="F23">
+        <v>277</v>
+      </c>
+      <c r="G23">
+        <v>278</v>
+      </c>
+      <c r="H23">
+        <v>279</v>
+      </c>
+      <c r="I23">
+        <v>280</v>
+      </c>
+      <c r="J23">
+        <v>281</v>
+      </c>
+      <c r="K23">
+        <v>282</v>
+      </c>
+      <c r="L23">
+        <v>283</v>
+      </c>
+      <c r="M23">
+        <v>284</v>
+      </c>
+      <c r="N23">
+        <v>285</v>
+      </c>
+      <c r="O23">
+        <v>286</v>
+      </c>
+      <c r="P23">
+        <v>287</v>
+      </c>
+      <c r="R23" s="5">
+        <v>17</v>
+      </c>
+      <c r="S23" s="10">
+        <f>IF(R23&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T23" s="8">
+        <f>R23*$S$4+U23</f>
+        <v>358</v>
+      </c>
+      <c r="U23" s="2">
+        <f>MIN($T$4,R23)</f>
+        <v>1</v>
+      </c>
+      <c r="V23" s="35">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="W23" s="36">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="X23" s="44">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Y23" s="44">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="Z23" s="36">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="AA23" s="37">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R24" s="5">
+        <v>18</v>
+      </c>
+      <c r="S24" s="10">
+        <f>IF(R24&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T24" s="8">
+        <f>R24*$S$4+U24</f>
+        <v>379</v>
+      </c>
+      <c r="U24" s="2">
+        <f>MIN($T$4,R24)</f>
+        <v>1</v>
+      </c>
+      <c r="V24" s="35">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="W24" s="36">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="X24" s="44">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="Y24" s="44">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="Z24" s="36">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="AA24" s="37">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R25" s="6">
+        <v>19</v>
+      </c>
+      <c r="S25" s="11">
+        <f>IF(R25&lt;$T$4,$S$4+1,$S$4)</f>
+        <v>21</v>
+      </c>
+      <c r="T25" s="9">
+        <f>R25*$S$4+U25</f>
+        <v>400</v>
+      </c>
+      <c r="U25" s="3">
+        <f>MIN($T$4,R25)</f>
+        <v>1</v>
+      </c>
+      <c r="V25" s="39">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="W25" s="40">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="X25" s="30">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="Y25" s="30">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="Z25" s="40">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="AA25" s="41">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A2:P3">
-    <cfRule type="expression" dxfId="4" priority="39">
-      <formula>AND(AND(A2&gt;=$D$10,A2&lt;$C$10+$D$10),AND(A2&lt;$B$5,$B$6&gt;=3))</formula>
+  <conditionalFormatting sqref="A6:P23">
+    <cfRule type="expression" dxfId="10" priority="4">
+      <formula>AND(AND(A6&gt;=$T$13,A6&lt;$S$13+$T$13),AND(A6&lt;$R$3,$R$4&gt;=8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="40">
-      <formula>AND(AND(A2&gt;=$D$9,A2&lt;$C$9+$D$9),AND(A2&lt;$B$5,$B$6&gt;=2))</formula>
+    <cfRule type="expression" dxfId="9" priority="6">
+      <formula>AND(AND(A6&gt;=$T$12,A6&lt;$S$12+$T$12),AND(A6&lt;$R$3,$R$4&gt;=7))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="41">
-      <formula>AND(AND(A2&gt;=$D$8,A2&lt;$D$8+$C$8),AND(A2&lt;$B$5,$B$6&gt;=1))</formula>
+    <cfRule type="expression" dxfId="8" priority="62">
+      <formula>AND(AND(A6&gt;=$T$11,A6&lt;$S$11+$T$11),AND(A6&lt;$R$3,$R$4&gt;=6))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>$B$5</formula>
+    <cfRule type="expression" dxfId="7" priority="63">
+      <formula>AND(AND(A6&gt;=$T$10,A6&lt;$S$10+$T$10),AND(A6&lt;$R$3,$R$4&gt;=5))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(AND(A2&gt;=$D$11,A2&lt;$C$11+$D$11),AND(A2&lt;$B$5,$B$6&gt;=4))</formula>
+    <cfRule type="expression" dxfId="6" priority="64">
+      <formula>AND(AND(A6&gt;=$T$9,A6&lt;$S$9+$T$9),AND(A6&lt;$R$3,$R$4&gt;=4))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="65" operator="equal">
+      <formula>$R$3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="66">
+      <formula>AND(AND(A6&gt;=$T$8,A6&lt;$S$8+$T$8),AND(A6&lt;$R$3,$R$4&gt;=3))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="67">
+      <formula>AND(AND(A6&gt;=$T$7,A6&lt;$S$7+$T$7),AND(A6&lt;$R$3,$R$4&gt;=2))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="68">
+      <formula>AND(AND(A6&gt;=$T$6,A6&lt;$T$6+$S$6),AND(A6&lt;$R$3,$R$4&gt;=1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V6:AA25">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$R$4-1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -937,20 +2819,20 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Spinner 1">
+            <control shapeId="1025" r:id="rId4" name="Drehfeld 1">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>581025</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:col>17</xdr:col>
+                    <xdr:colOff>579120</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>752475</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:col>17</xdr:col>
+                    <xdr:colOff>754380</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>259080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -959,20 +2841,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Spinner 2">
+            <control shapeId="1026" r:id="rId5" name="Drehfeld 2">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>4</xdr:row>
+                    <xdr:col>17</xdr:col>
+                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>266700</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>1</xdr:col>
+                    <xdr:col>17</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>259080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>